<commit_message>
Updated self city airport data
</commit_message>
<xml_diff>
--- a/dddmDEMO/Final_ScoresUpdatedColumn.xlsx
+++ b/dddmDEMO/Final_ScoresUpdatedColumn.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="252" uniqueCount="173">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="254" uniqueCount="175">
   <si>
     <t>state</t>
   </si>
@@ -199,6 +199,9 @@
     <t>Wisconsin</t>
   </si>
   <si>
+    <t xml:space="preserve">Washington D.C. </t>
+  </si>
+  <si>
     <t>Birmingham – Alabama</t>
   </si>
   <si>
@@ -529,10 +532,13 @@
     <t>Northern Virginia – Virginia</t>
   </si>
   <si>
-    <t>Milwaukee – Virginia</t>
-  </si>
-  <si>
-    <t>Madison – Virginia</t>
+    <t>Milwaukee – Wisconsin</t>
+  </si>
+  <si>
+    <t>Madison – Wisconsin</t>
+  </si>
+  <si>
+    <t>Washington D.C.</t>
   </si>
 </sst>
 </file>
@@ -890,7 +896,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AC113"/>
+  <dimension ref="A1:AC114"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -990,7 +996,7 @@
         <v>28</v>
       </c>
       <c r="C2" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="D2" t="b">
         <v>0</v>
@@ -1068,7 +1074,7 @@
         <v>6</v>
       </c>
       <c r="AC2">
-        <v>4.18671549506606</v>
+        <v>4.210556481126316</v>
       </c>
     </row>
     <row r="3" spans="1:29">
@@ -1079,7 +1085,7 @@
         <v>29</v>
       </c>
       <c r="C3" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="D3" t="b">
         <v>0</v>
@@ -1157,7 +1163,7 @@
         <v>0</v>
       </c>
       <c r="AC3">
-        <v>3.98528939966624</v>
+        <v>3.909895722116946</v>
       </c>
     </row>
     <row r="4" spans="1:29">
@@ -1168,7 +1174,7 @@
         <v>30</v>
       </c>
       <c r="C4" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="D4" t="b">
         <v>0</v>
@@ -1246,7 +1252,7 @@
         <v>3</v>
       </c>
       <c r="AC4">
-        <v>3.68327172248722</v>
+        <v>3.695337173650969</v>
       </c>
     </row>
     <row r="5" spans="1:29">
@@ -1257,7 +1263,7 @@
         <v>31</v>
       </c>
       <c r="C5" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="D5" t="b">
         <v>0</v>
@@ -1335,7 +1341,7 @@
         <v>0.73</v>
       </c>
       <c r="AC5">
-        <v>3.81368914662841</v>
+        <v>3.838383078751985</v>
       </c>
     </row>
     <row r="6" spans="1:29">
@@ -1346,7 +1352,7 @@
         <v>31</v>
       </c>
       <c r="C6" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="D6" t="b">
         <v>1</v>
@@ -1424,7 +1430,7 @@
         <v>2</v>
       </c>
       <c r="AC6">
-        <v>6.69436390241473</v>
+        <v>6.828378372877175</v>
       </c>
     </row>
     <row r="7" spans="1:29">
@@ -1435,7 +1441,7 @@
         <v>31</v>
       </c>
       <c r="C7" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="D7" t="b">
         <v>0</v>
@@ -1513,7 +1519,7 @@
         <v>0.5</v>
       </c>
       <c r="AC7">
-        <v>6.00048450478591</v>
+        <v>6.086697918047746</v>
       </c>
     </row>
     <row r="8" spans="1:29">
@@ -1524,7 +1530,7 @@
         <v>31</v>
       </c>
       <c r="C8" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="D8" t="b">
         <v>0</v>
@@ -1602,7 +1608,7 @@
         <v>1</v>
       </c>
       <c r="AC8">
-        <v>6.19485934183891</v>
+        <v>6.232130758331659</v>
       </c>
     </row>
     <row r="9" spans="1:29">
@@ -1613,7 +1619,7 @@
         <v>31</v>
       </c>
       <c r="C9" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="D9" t="b">
         <v>0</v>
@@ -1691,7 +1697,7 @@
         <v>0.5</v>
       </c>
       <c r="AC9">
-        <v>7.11787731657328</v>
+        <v>7.203942109422554</v>
       </c>
     </row>
     <row r="10" spans="1:29">
@@ -1702,7 +1708,7 @@
         <v>31</v>
       </c>
       <c r="C10" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="D10" t="b">
         <v>0</v>
@@ -1738,7 +1744,7 @@
         <v>0</v>
       </c>
       <c r="O10">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="P10">
         <v>0</v>
@@ -1780,7 +1786,7 @@
         <v>1</v>
       </c>
       <c r="AC10">
-        <v>5.83365154736528</v>
+        <v>6.708039749468196</v>
       </c>
     </row>
     <row r="11" spans="1:29">
@@ -1791,7 +1797,7 @@
         <v>31</v>
       </c>
       <c r="C11" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="D11" t="b">
         <v>0</v>
@@ -1869,7 +1875,7 @@
         <v>1.5</v>
       </c>
       <c r="AC11">
-        <v>6.16822355806006</v>
+        <v>6.169641932022943</v>
       </c>
     </row>
     <row r="12" spans="1:29">
@@ -1880,7 +1886,7 @@
         <v>31</v>
       </c>
       <c r="C12" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="D12" t="b">
         <v>0</v>
@@ -1958,7 +1964,7 @@
         <v>1</v>
       </c>
       <c r="AC12">
-        <v>3.74521736211462</v>
+        <v>3.722322220335927</v>
       </c>
     </row>
     <row r="13" spans="1:29">
@@ -1969,7 +1975,7 @@
         <v>31</v>
       </c>
       <c r="C13" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="D13" t="b">
         <v>0</v>
@@ -2047,7 +2053,7 @@
         <v>3</v>
       </c>
       <c r="AC13">
-        <v>3.65959857658755</v>
+        <v>3.673231583640857</v>
       </c>
     </row>
     <row r="14" spans="1:29">
@@ -2058,7 +2064,7 @@
         <v>32</v>
       </c>
       <c r="C14" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="D14" t="b">
         <v>1</v>
@@ -2136,7 +2142,7 @@
         <v>4.75</v>
       </c>
       <c r="AC14">
-        <v>6.77047297868889</v>
+        <v>6.834595556599855</v>
       </c>
     </row>
     <row r="15" spans="1:29">
@@ -2147,7 +2153,7 @@
         <v>33</v>
       </c>
       <c r="C15" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="D15" t="b">
         <v>0</v>
@@ -2225,7 +2231,7 @@
         <v>0</v>
       </c>
       <c r="AC15">
-        <v>4.85955511875319</v>
+        <v>4.848975541471533</v>
       </c>
     </row>
     <row r="16" spans="1:29">
@@ -2236,7 +2242,7 @@
         <v>33</v>
       </c>
       <c r="C16" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="D16" t="b">
         <v>0</v>
@@ -2314,7 +2320,7 @@
         <v>0</v>
       </c>
       <c r="AC16">
-        <v>4.44995033121616</v>
+        <v>4.450346307838432</v>
       </c>
     </row>
     <row r="17" spans="1:29">
@@ -2325,7 +2331,7 @@
         <v>33</v>
       </c>
       <c r="C17" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="D17" t="b">
         <v>0</v>
@@ -2403,7 +2409,7 @@
         <v>0</v>
       </c>
       <c r="AC17">
-        <v>4.86222323383665</v>
+        <v>4.875435759982659</v>
       </c>
     </row>
     <row r="18" spans="1:29">
@@ -2414,7 +2420,7 @@
         <v>33</v>
       </c>
       <c r="C18" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="D18" t="b">
         <v>0</v>
@@ -2492,7 +2498,7 @@
         <v>0</v>
       </c>
       <c r="AC18">
-        <v>3.68678384651249</v>
+        <v>3.676116834841885</v>
       </c>
     </row>
     <row r="19" spans="1:29">
@@ -2503,7 +2509,7 @@
         <v>33</v>
       </c>
       <c r="C19" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="D19" t="b">
         <v>0</v>
@@ -2581,7 +2587,7 @@
         <v>0</v>
       </c>
       <c r="AC19">
-        <v>4.12283713757958</v>
+        <v>4.136121377979959</v>
       </c>
     </row>
     <row r="20" spans="1:29">
@@ -2592,7 +2598,7 @@
         <v>34</v>
       </c>
       <c r="C20" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="D20" t="b">
         <v>1</v>
@@ -2670,7 +2676,7 @@
         <v>1</v>
       </c>
       <c r="AC20">
-        <v>6.73765671342299</v>
+        <v>6.706682359940232</v>
       </c>
     </row>
     <row r="21" spans="1:29">
@@ -2681,7 +2687,7 @@
         <v>34</v>
       </c>
       <c r="C21" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="D21" t="b">
         <v>0</v>
@@ -2759,7 +2765,7 @@
         <v>1</v>
       </c>
       <c r="AC21">
-        <v>6.4594465662515</v>
+        <v>6.416861987488036</v>
       </c>
     </row>
     <row r="22" spans="1:29">
@@ -2770,7 +2776,7 @@
         <v>34</v>
       </c>
       <c r="C22" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="D22" t="b">
         <v>0</v>
@@ -2848,7 +2854,7 @@
         <v>0.5</v>
       </c>
       <c r="AC22">
-        <v>6.97824803963936</v>
+        <v>6.983575932577238</v>
       </c>
     </row>
     <row r="23" spans="1:29">
@@ -2859,7 +2865,7 @@
         <v>35</v>
       </c>
       <c r="C23" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="D23" t="b">
         <v>1</v>
@@ -2937,7 +2943,7 @@
         <v>4.9</v>
       </c>
       <c r="AC23">
-        <v>6.43558217026719</v>
+        <v>6.428886148937228</v>
       </c>
     </row>
     <row r="24" spans="1:29">
@@ -2948,7 +2954,7 @@
         <v>35</v>
       </c>
       <c r="C24" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="D24" t="b">
         <v>0</v>
@@ -3026,7 +3032,7 @@
         <v>4.9</v>
       </c>
       <c r="AC24">
-        <v>3.78937363862026</v>
+        <v>3.784265585097816</v>
       </c>
     </row>
     <row r="25" spans="1:29">
@@ -3037,7 +3043,7 @@
         <v>36</v>
       </c>
       <c r="C25" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="D25" t="b">
         <v>1</v>
@@ -3115,7 +3121,7 @@
         <v>4</v>
       </c>
       <c r="AC25">
-        <v>7.16510454469634</v>
+        <v>7.135734103078507</v>
       </c>
     </row>
     <row r="26" spans="1:29">
@@ -3126,7 +3132,7 @@
         <v>37</v>
       </c>
       <c r="C26" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="D26" t="b">
         <v>1</v>
@@ -3204,7 +3210,7 @@
         <v>0</v>
       </c>
       <c r="AC26">
-        <v>5.79120427541609</v>
+        <v>5.80769364641284</v>
       </c>
     </row>
     <row r="27" spans="1:29">
@@ -3215,7 +3221,7 @@
         <v>37</v>
       </c>
       <c r="C27" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="D27" t="b">
         <v>0</v>
@@ -3293,7 +3299,7 @@
         <v>0</v>
       </c>
       <c r="AC27">
-        <v>3.91032164182633</v>
+        <v>3.934666470541204</v>
       </c>
     </row>
     <row r="28" spans="1:29">
@@ -3304,7 +3310,7 @@
         <v>38</v>
       </c>
       <c r="C28" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="D28" t="b">
         <v>0</v>
@@ -3382,7 +3388,7 @@
         <v>0</v>
       </c>
       <c r="AC28">
-        <v>5.21264360966847</v>
+        <v>5.22595302578463</v>
       </c>
     </row>
     <row r="29" spans="1:29">
@@ -3393,7 +3399,7 @@
         <v>39</v>
       </c>
       <c r="C29" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="D29" t="b">
         <v>0</v>
@@ -3471,7 +3477,7 @@
         <v>1</v>
       </c>
       <c r="AC29">
-        <v>5.65644569939801</v>
+        <v>5.703339386727711</v>
       </c>
     </row>
     <row r="30" spans="1:29">
@@ -3482,7 +3488,7 @@
         <v>40</v>
       </c>
       <c r="C30" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="D30" t="b">
         <v>0</v>
@@ -3560,7 +3566,7 @@
         <v>0</v>
       </c>
       <c r="AC30">
-        <v>5.2104634555344</v>
+        <v>5.191366243965748</v>
       </c>
     </row>
     <row r="31" spans="1:29">
@@ -3571,7 +3577,7 @@
         <v>41</v>
       </c>
       <c r="C31" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="D31" t="b">
         <v>0</v>
@@ -3649,7 +3655,7 @@
         <v>0</v>
       </c>
       <c r="AC31">
-        <v>4.83242298770305</v>
+        <v>4.788363843523755</v>
       </c>
     </row>
     <row r="32" spans="1:29">
@@ -3660,7 +3666,7 @@
         <v>41</v>
       </c>
       <c r="C32" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="D32" t="b">
         <v>0</v>
@@ -3738,7 +3744,7 @@
         <v>0</v>
       </c>
       <c r="AC32">
-        <v>4.99013232066998</v>
+        <v>4.946177306283944</v>
       </c>
     </row>
     <row r="33" spans="1:29">
@@ -3749,7 +3755,7 @@
         <v>42</v>
       </c>
       <c r="C33" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="D33" t="b">
         <v>0</v>
@@ -3827,7 +3833,7 @@
         <v>0</v>
       </c>
       <c r="AC33">
-        <v>5.80876668147899</v>
+        <v>5.857996245439912</v>
       </c>
     </row>
     <row r="34" spans="1:29">
@@ -3838,7 +3844,7 @@
         <v>42</v>
       </c>
       <c r="C34" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="D34" t="b">
         <v>0</v>
@@ -3916,7 +3922,7 @@
         <v>0</v>
       </c>
       <c r="AC34">
-        <v>3.91527084873814</v>
+        <v>3.965614561003554</v>
       </c>
     </row>
     <row r="35" spans="1:29">
@@ -3927,7 +3933,7 @@
         <v>42</v>
       </c>
       <c r="C35" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="D35" t="b">
         <v>1</v>
@@ -4005,7 +4011,7 @@
         <v>0</v>
       </c>
       <c r="AC35">
-        <v>4.78531597479261</v>
+        <v>4.83575302325406</v>
       </c>
     </row>
     <row r="36" spans="1:29">
@@ -4016,7 +4022,7 @@
         <v>43</v>
       </c>
       <c r="C36" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="D36" t="b">
         <v>0</v>
@@ -4094,7 +4100,7 @@
         <v>0</v>
       </c>
       <c r="AC36">
-        <v>5.93485719622129</v>
+        <v>5.977973324415419</v>
       </c>
     </row>
     <row r="37" spans="1:29">
@@ -4105,7 +4111,7 @@
         <v>43</v>
       </c>
       <c r="C37" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="D37" t="b">
         <v>0</v>
@@ -4183,7 +4189,7 @@
         <v>0</v>
       </c>
       <c r="AC37">
-        <v>6.31504805416012</v>
+        <v>6.304302388920509</v>
       </c>
     </row>
     <row r="38" spans="1:29">
@@ -4194,7 +4200,7 @@
         <v>43</v>
       </c>
       <c r="C38" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="D38" t="b">
         <v>1</v>
@@ -4272,7 +4278,7 @@
         <v>0</v>
       </c>
       <c r="AC38">
-        <v>7.39926890974049</v>
+        <v>7.439842604892244</v>
       </c>
     </row>
     <row r="39" spans="1:29">
@@ -4283,7 +4289,7 @@
         <v>43</v>
       </c>
       <c r="C39" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="D39" t="b">
         <v>0</v>
@@ -4361,7 +4367,7 @@
         <v>0</v>
       </c>
       <c r="AC39">
-        <v>5.88066833468738</v>
+        <v>5.924148177686354</v>
       </c>
     </row>
     <row r="40" spans="1:29">
@@ -4372,7 +4378,7 @@
         <v>43</v>
       </c>
       <c r="C40" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="D40" t="b">
         <v>0</v>
@@ -4450,7 +4456,7 @@
         <v>0</v>
       </c>
       <c r="AC40">
-        <v>6.03178255126555</v>
+        <v>6.074985769619514</v>
       </c>
     </row>
     <row r="41" spans="1:29">
@@ -4461,7 +4467,7 @@
         <v>43</v>
       </c>
       <c r="C41" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="D41" t="b">
         <v>0</v>
@@ -4539,7 +4545,7 @@
         <v>0</v>
       </c>
       <c r="AC41">
-        <v>5.73673854780142</v>
+        <v>5.780083530488447</v>
       </c>
     </row>
     <row r="42" spans="1:29">
@@ -4550,7 +4556,7 @@
         <v>43</v>
       </c>
       <c r="C42" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="D42" t="b">
         <v>0</v>
@@ -4628,7 +4634,7 @@
         <v>0</v>
       </c>
       <c r="AC42">
-        <v>5.22390938165581</v>
+        <v>5.267078630486325</v>
       </c>
     </row>
     <row r="43" spans="1:29">
@@ -4639,7 +4645,7 @@
         <v>43</v>
       </c>
       <c r="C43" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="D43" t="b">
         <v>0</v>
@@ -4717,7 +4723,7 @@
         <v>0</v>
       </c>
       <c r="AC43">
-        <v>4.59350735507825</v>
+        <v>4.636608631874995</v>
       </c>
     </row>
     <row r="44" spans="1:29">
@@ -4728,7 +4734,7 @@
         <v>43</v>
       </c>
       <c r="C44" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="D44" t="b">
         <v>0</v>
@@ -4806,7 +4812,7 @@
         <v>0</v>
       </c>
       <c r="AC44">
-        <v>5.59387636300598</v>
+        <v>5.637078138950337</v>
       </c>
     </row>
     <row r="45" spans="1:29">
@@ -4817,7 +4823,7 @@
         <v>43</v>
       </c>
       <c r="C45" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="D45" t="b">
         <v>0</v>
@@ -4895,7 +4901,7 @@
         <v>0</v>
       </c>
       <c r="AC45">
-        <v>4.38081072144048</v>
+        <v>4.423665228815809</v>
       </c>
     </row>
     <row r="46" spans="1:29">
@@ -4906,7 +4912,7 @@
         <v>43</v>
       </c>
       <c r="C46" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="D46" t="b">
         <v>0</v>
@@ -4984,7 +4990,7 @@
         <v>0</v>
       </c>
       <c r="AC46">
-        <v>5.30427371426373</v>
+        <v>5.347490534131101</v>
       </c>
     </row>
     <row r="47" spans="1:29">
@@ -4995,7 +5001,7 @@
         <v>43</v>
       </c>
       <c r="C47" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="D47" t="b">
         <v>0</v>
@@ -5073,7 +5079,7 @@
         <v>0</v>
       </c>
       <c r="AC47">
-        <v>6.06691836295982</v>
+        <v>6.110264401016741</v>
       </c>
     </row>
     <row r="48" spans="1:29">
@@ -5084,7 +5090,7 @@
         <v>43</v>
       </c>
       <c r="C48" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="D48" t="b">
         <v>0</v>
@@ -5162,7 +5168,7 @@
         <v>0</v>
       </c>
       <c r="AC48">
-        <v>5.83948670585595</v>
+        <v>5.882931701281661</v>
       </c>
     </row>
     <row r="49" spans="1:29">
@@ -5173,7 +5179,7 @@
         <v>43</v>
       </c>
       <c r="C49" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="D49" t="b">
         <v>0</v>
@@ -5251,7 +5257,7 @@
         <v>0</v>
       </c>
       <c r="AC49">
-        <v>5.52615204214626</v>
+        <v>5.56948303250207</v>
       </c>
     </row>
     <row r="50" spans="1:29">
@@ -5262,7 +5268,7 @@
         <v>43</v>
       </c>
       <c r="C50" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="D50" t="b">
         <v>0</v>
@@ -5340,7 +5346,7 @@
         <v>0</v>
       </c>
       <c r="AC50">
-        <v>6.01197167711705</v>
+        <v>6.055059996397329</v>
       </c>
     </row>
     <row r="51" spans="1:29">
@@ -5351,7 +5357,7 @@
         <v>43</v>
       </c>
       <c r="C51" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="D51" t="b">
         <v>0</v>
@@ -5429,7 +5435,7 @@
         <v>0</v>
       </c>
       <c r="AC51">
-        <v>5.81446714092538</v>
+        <v>5.857668916869738</v>
       </c>
     </row>
     <row r="52" spans="1:29">
@@ -5440,7 +5446,7 @@
         <v>43</v>
       </c>
       <c r="C52" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="D52" t="b">
         <v>0</v>
@@ -5518,7 +5524,7 @@
         <v>0</v>
       </c>
       <c r="AC52">
-        <v>5.63936493250963</v>
+        <v>5.682759147642267</v>
       </c>
     </row>
     <row r="53" spans="1:29">
@@ -5529,7 +5535,7 @@
         <v>43</v>
       </c>
       <c r="C53" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="D53" t="b">
         <v>0</v>
@@ -5607,7 +5613,7 @@
         <v>0</v>
       </c>
       <c r="AC53">
-        <v>5.11626709230443</v>
+        <v>5.159511682181955</v>
       </c>
     </row>
     <row r="54" spans="1:29">
@@ -5618,7 +5624,7 @@
         <v>43</v>
       </c>
       <c r="C54" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="D54" t="b">
         <v>0</v>
@@ -5696,7 +5702,7 @@
         <v>0</v>
       </c>
       <c r="AC54">
-        <v>5.78050901000989</v>
+        <v>5.823882639033572</v>
       </c>
     </row>
     <row r="55" spans="1:29">
@@ -5707,7 +5713,7 @@
         <v>43</v>
       </c>
       <c r="C55" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="D55" t="b">
         <v>0</v>
@@ -5785,7 +5791,7 @@
         <v>0</v>
       </c>
       <c r="AC55">
-        <v>6.02449892309757</v>
+        <v>6.067805355323006</v>
       </c>
     </row>
     <row r="56" spans="1:29">
@@ -5796,7 +5802,7 @@
         <v>43</v>
       </c>
       <c r="C56" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="D56" t="b">
         <v>0</v>
@@ -5874,7 +5880,7 @@
         <v>0</v>
       </c>
       <c r="AC56">
-        <v>5.63855692656007</v>
+        <v>5.681858920048636</v>
       </c>
     </row>
     <row r="57" spans="1:29">
@@ -5885,7 +5891,7 @@
         <v>43</v>
       </c>
       <c r="C57" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="D57" t="b">
         <v>0</v>
@@ -5963,7 +5969,7 @@
         <v>0</v>
       </c>
       <c r="AC57">
-        <v>5.70555318013118</v>
+        <v>5.748773984490281</v>
       </c>
     </row>
     <row r="58" spans="1:29">
@@ -5974,7 +5980,7 @@
         <v>43</v>
       </c>
       <c r="C58" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="D58" t="b">
         <v>0</v>
@@ -6052,7 +6058,7 @@
         <v>0</v>
       </c>
       <c r="AC58">
-        <v>5.82490837717389</v>
+        <v>5.868345406239691</v>
       </c>
     </row>
     <row r="59" spans="1:29">
@@ -6063,7 +6069,7 @@
         <v>43</v>
       </c>
       <c r="C59" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="D59" t="b">
         <v>0</v>
@@ -6141,7 +6147,7 @@
         <v>0</v>
       </c>
       <c r="AC59">
-        <v>5.83243798612393</v>
+        <v>5.875649276275656</v>
       </c>
     </row>
     <row r="60" spans="1:29">
@@ -6152,7 +6158,7 @@
         <v>44</v>
       </c>
       <c r="C60" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="D60" t="b">
         <v>0</v>
@@ -6230,7 +6236,7 @@
         <v>0</v>
       </c>
       <c r="AC60">
-        <v>5.78005455364479</v>
+        <v>5.772370510241812</v>
       </c>
     </row>
     <row r="61" spans="1:29">
@@ -6241,7 +6247,7 @@
         <v>44</v>
       </c>
       <c r="C61" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="D61" t="b">
         <v>0</v>
@@ -6319,7 +6325,7 @@
         <v>0</v>
       </c>
       <c r="AC61">
-        <v>5.69260091973231</v>
+        <v>5.684048590699295</v>
       </c>
     </row>
     <row r="62" spans="1:29">
@@ -6330,7 +6336,7 @@
         <v>45</v>
       </c>
       <c r="C62" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="D62" t="b">
         <v>0</v>
@@ -6408,7 +6414,7 @@
         <v>0.9</v>
       </c>
       <c r="AC62">
-        <v>6.82887690279436</v>
+        <v>6.88114723571185</v>
       </c>
     </row>
     <row r="63" spans="1:29">
@@ -6419,7 +6425,7 @@
         <v>46</v>
       </c>
       <c r="C63" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="D63" t="b">
         <v>0</v>
@@ -6497,7 +6503,7 @@
         <v>4.45</v>
       </c>
       <c r="AC63">
-        <v>6.62705262719321</v>
+        <v>6.726563284170673</v>
       </c>
     </row>
     <row r="64" spans="1:29">
@@ -6508,7 +6514,7 @@
         <v>46</v>
       </c>
       <c r="C64" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="D64" t="b">
         <v>0</v>
@@ -6586,7 +6592,7 @@
         <v>4.13</v>
       </c>
       <c r="AC64">
-        <v>5.90464742972868</v>
+        <v>5.929262969555773</v>
       </c>
     </row>
     <row r="65" spans="1:29">
@@ -6597,7 +6603,7 @@
         <v>47</v>
       </c>
       <c r="C65" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="D65" t="b">
         <v>0</v>
@@ -6675,7 +6681,7 @@
         <v>1.5</v>
       </c>
       <c r="AC65">
-        <v>6.06318671149544</v>
+        <v>6.089455796111457</v>
       </c>
     </row>
     <row r="66" spans="1:29">
@@ -6686,7 +6692,7 @@
         <v>48</v>
       </c>
       <c r="C66" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="D66" t="b">
         <v>0</v>
@@ -6764,7 +6770,7 @@
         <v>1.3</v>
       </c>
       <c r="AC66">
-        <v>6.42942442230409</v>
+        <v>6.518858170534222</v>
       </c>
     </row>
     <row r="67" spans="1:29">
@@ -6775,7 +6781,7 @@
         <v>49</v>
       </c>
       <c r="C67" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="D67" t="b">
         <v>0</v>
@@ -6853,7 +6859,7 @@
         <v>0</v>
       </c>
       <c r="AC67">
-        <v>5.10326352988842</v>
+        <v>5.089561283258011</v>
       </c>
     </row>
     <row r="68" spans="1:29">
@@ -6864,7 +6870,7 @@
         <v>49</v>
       </c>
       <c r="C68" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="D68" t="b">
         <v>0</v>
@@ -6942,7 +6948,7 @@
         <v>0</v>
       </c>
       <c r="AC68">
-        <v>5.35025326178947</v>
+        <v>5.336657077195814</v>
       </c>
     </row>
     <row r="69" spans="1:29">
@@ -6953,7 +6959,7 @@
         <v>12</v>
       </c>
       <c r="C69" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="D69" t="b">
         <v>0</v>
@@ -7031,7 +7037,7 @@
         <v>4.75</v>
       </c>
       <c r="AC69">
-        <v>5.59148887294038</v>
+        <v>5.558307096702853</v>
       </c>
     </row>
     <row r="70" spans="1:29">
@@ -7042,7 +7048,7 @@
         <v>12</v>
       </c>
       <c r="C70" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="D70" t="b">
         <v>0</v>
@@ -7120,7 +7126,7 @@
         <v>4.75</v>
       </c>
       <c r="AC70">
-        <v>5.7662003120548</v>
+        <v>5.766109690518703</v>
       </c>
     </row>
     <row r="71" spans="1:29">
@@ -7131,7 +7137,7 @@
         <v>12</v>
       </c>
       <c r="C71" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="D71" t="b">
         <v>0</v>
@@ -7209,7 +7215,7 @@
         <v>4.75</v>
       </c>
       <c r="AC71">
-        <v>4.80756487782957</v>
+        <v>4.807913876969971</v>
       </c>
     </row>
     <row r="72" spans="1:29">
@@ -7220,7 +7226,7 @@
         <v>12</v>
       </c>
       <c r="C72" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="D72" t="b">
         <v>1</v>
@@ -7253,7 +7259,7 @@
         <v>4</v>
       </c>
       <c r="N72">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="O72">
         <v>5</v>
@@ -7298,7 +7304,7 @@
         <v>4.75</v>
       </c>
       <c r="AC72">
-        <v>6.893985301555</v>
+        <v>7.987934718712288</v>
       </c>
     </row>
     <row r="73" spans="1:29">
@@ -7309,7 +7315,7 @@
         <v>12</v>
       </c>
       <c r="C73" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="D73" t="b">
         <v>0</v>
@@ -7387,7 +7393,7 @@
         <v>4.75</v>
       </c>
       <c r="AC73">
-        <v>4.99290545687101</v>
+        <v>5.114018997689896</v>
       </c>
     </row>
     <row r="74" spans="1:29">
@@ -7398,7 +7404,7 @@
         <v>12</v>
       </c>
       <c r="C74" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="D74" t="b">
         <v>0</v>
@@ -7476,7 +7482,7 @@
         <v>4.75</v>
       </c>
       <c r="AC74">
-        <v>5.04309276571919</v>
+        <v>5.164282718870368</v>
       </c>
     </row>
     <row r="75" spans="1:29">
@@ -7487,7 +7493,7 @@
         <v>12</v>
       </c>
       <c r="C75" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="D75" t="b">
         <v>0</v>
@@ -7565,7 +7571,7 @@
         <v>4.75</v>
       </c>
       <c r="AC75">
-        <v>5.23650660321074</v>
+        <v>5.203642832574967</v>
       </c>
     </row>
     <row r="76" spans="1:29">
@@ -7576,7 +7582,7 @@
         <v>50</v>
       </c>
       <c r="C76" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="D76" t="b">
         <v>0</v>
@@ -7654,7 +7660,7 @@
         <v>2</v>
       </c>
       <c r="AC76">
-        <v>5.97936659933646</v>
+        <v>5.956988646227575</v>
       </c>
     </row>
     <row r="77" spans="1:29">
@@ -7665,7 +7671,7 @@
         <v>50</v>
       </c>
       <c r="C77" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="D77" t="b">
         <v>0</v>
@@ -7743,7 +7749,7 @@
         <v>2.5</v>
       </c>
       <c r="AC77">
-        <v>5.45452064315424</v>
+        <v>5.411660473860315</v>
       </c>
     </row>
     <row r="78" spans="1:29">
@@ -7754,7 +7760,7 @@
         <v>50</v>
       </c>
       <c r="C78" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="D78" t="b">
         <v>1</v>
@@ -7832,7 +7838,7 @@
         <v>2</v>
       </c>
       <c r="AC78">
-        <v>7.75373386027154</v>
+        <v>7.781635816195867</v>
       </c>
     </row>
     <row r="79" spans="1:29">
@@ -7843,7 +7849,7 @@
         <v>50</v>
       </c>
       <c r="C79" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="D79" t="b">
         <v>0</v>
@@ -7921,7 +7927,7 @@
         <v>2</v>
       </c>
       <c r="AC79">
-        <v>5.00930011213421</v>
+        <v>4.966999288577204</v>
       </c>
     </row>
     <row r="80" spans="1:29">
@@ -7932,7 +7938,7 @@
         <v>51</v>
       </c>
       <c r="C80" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="D80" t="b">
         <v>0</v>
@@ -8010,7 +8016,7 @@
         <v>2.25</v>
       </c>
       <c r="AC80">
-        <v>4.80211931195861</v>
+        <v>4.76963244787856</v>
       </c>
     </row>
     <row r="81" spans="1:29">
@@ -8021,7 +8027,7 @@
         <v>51</v>
       </c>
       <c r="C81" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="D81" t="b">
         <v>0</v>
@@ -8099,7 +8105,7 @@
         <v>2.25</v>
       </c>
       <c r="AC81">
-        <v>5.87985058237722</v>
+        <v>5.860564717361457</v>
       </c>
     </row>
     <row r="82" spans="1:29">
@@ -8110,7 +8116,7 @@
         <v>51</v>
       </c>
       <c r="C82" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="D82" t="b">
         <v>1</v>
@@ -8188,7 +8194,7 @@
         <v>1.75</v>
       </c>
       <c r="AC82">
-        <v>6.71879272150149</v>
+        <v>6.673934739257777</v>
       </c>
     </row>
     <row r="83" spans="1:29">
@@ -8199,7 +8205,7 @@
         <v>52</v>
       </c>
       <c r="C83" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="D83" t="b">
         <v>0</v>
@@ -8277,7 +8283,7 @@
         <v>4.02</v>
       </c>
       <c r="AC83">
-        <v>4.52908488968536</v>
+        <v>4.541809156308467</v>
       </c>
     </row>
     <row r="84" spans="1:29">
@@ -8288,7 +8294,7 @@
         <v>52</v>
       </c>
       <c r="C84" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="D84" t="b">
         <v>0</v>
@@ -8366,7 +8372,7 @@
         <v>3.88</v>
       </c>
       <c r="AC84">
-        <v>5.77902457318343</v>
+        <v>5.802597336979916</v>
       </c>
     </row>
     <row r="85" spans="1:29">
@@ -8377,7 +8383,7 @@
         <v>53</v>
       </c>
       <c r="C85" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="D85" t="b">
         <v>0</v>
@@ -8455,7 +8461,7 @@
         <v>0</v>
       </c>
       <c r="AC85">
-        <v>7.05091817672516</v>
+        <v>7.138085861762434</v>
       </c>
     </row>
     <row r="86" spans="1:29">
@@ -8466,7 +8472,7 @@
         <v>54</v>
       </c>
       <c r="C86" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="D86" t="b">
         <v>1</v>
@@ -8544,7 +8550,7 @@
         <v>1</v>
       </c>
       <c r="AC86">
-        <v>5.94788361976171</v>
+        <v>5.916056568413392</v>
       </c>
     </row>
     <row r="87" spans="1:29">
@@ -8555,7 +8561,7 @@
         <v>54</v>
       </c>
       <c r="C87" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="D87" t="b">
         <v>1</v>
@@ -8633,7 +8639,7 @@
         <v>2</v>
       </c>
       <c r="AC87">
-        <v>6.57613803087775</v>
+        <v>6.61612822795899</v>
       </c>
     </row>
     <row r="88" spans="1:29">
@@ -8644,7 +8650,7 @@
         <v>54</v>
       </c>
       <c r="C88" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="D88" t="b">
         <v>0</v>
@@ -8722,7 +8728,7 @@
         <v>1</v>
       </c>
       <c r="AC88">
-        <v>4.96533648530203</v>
+        <v>4.965896600313615</v>
       </c>
     </row>
     <row r="89" spans="1:29">
@@ -8733,7 +8739,7 @@
         <v>54</v>
       </c>
       <c r="C89" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="D89" t="b">
         <v>0</v>
@@ -8811,7 +8817,7 @@
         <v>1</v>
       </c>
       <c r="AC89">
-        <v>4.43426301880687</v>
+        <v>4.423561601949645</v>
       </c>
     </row>
     <row r="90" spans="1:29">
@@ -8822,7 +8828,7 @@
         <v>54</v>
       </c>
       <c r="C90" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="D90" t="b">
         <v>0</v>
@@ -8900,7 +8906,7 @@
         <v>1</v>
       </c>
       <c r="AC90">
-        <v>4.46110802416636</v>
+        <v>4.450491917916222</v>
       </c>
     </row>
     <row r="91" spans="1:29">
@@ -8911,7 +8917,7 @@
         <v>54</v>
       </c>
       <c r="C91" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="D91" t="b">
         <v>0</v>
@@ -8989,7 +8995,7 @@
         <v>1</v>
       </c>
       <c r="AC91">
-        <v>3.40043176044931</v>
+        <v>3.424828500481773</v>
       </c>
     </row>
     <row r="92" spans="1:29">
@@ -9000,7 +9006,7 @@
         <v>55</v>
       </c>
       <c r="C92" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="D92" t="b">
         <v>0</v>
@@ -9078,7 +9084,7 @@
         <v>0</v>
       </c>
       <c r="AC92">
-        <v>6.20848754151411</v>
+        <v>6.208741055422141</v>
       </c>
     </row>
     <row r="93" spans="1:29">
@@ -9089,7 +9095,7 @@
         <v>55</v>
       </c>
       <c r="C93" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="D93" t="b">
         <v>0</v>
@@ -9167,7 +9173,7 @@
         <v>0</v>
       </c>
       <c r="AC93">
-        <v>5.64742498169566</v>
+        <v>5.647850531824542</v>
       </c>
     </row>
     <row r="94" spans="1:29">
@@ -9178,7 +9184,7 @@
         <v>55</v>
       </c>
       <c r="C94" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="D94" t="b">
         <v>0</v>
@@ -9256,7 +9262,7 @@
         <v>0</v>
       </c>
       <c r="AC94">
-        <v>5.84778677893988</v>
+        <v>5.84792104688896</v>
       </c>
     </row>
     <row r="95" spans="1:29">
@@ -9267,7 +9273,7 @@
         <v>55</v>
       </c>
       <c r="C95" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="D95" t="b">
         <v>0</v>
@@ -9345,7 +9351,7 @@
         <v>0</v>
       </c>
       <c r="AC95">
-        <v>5.00917773668047</v>
+        <v>5.009639929046132</v>
       </c>
     </row>
     <row r="96" spans="1:29">
@@ -9356,7 +9362,7 @@
         <v>55</v>
       </c>
       <c r="C96" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="D96" t="b">
         <v>0</v>
@@ -9434,7 +9440,7 @@
         <v>0</v>
       </c>
       <c r="AC96">
-        <v>5.68646815940822</v>
+        <v>5.687074126322987</v>
       </c>
     </row>
     <row r="97" spans="1:29">
@@ -9445,7 +9451,7 @@
         <v>55</v>
       </c>
       <c r="C97" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="D97" t="b">
         <v>0</v>
@@ -9523,7 +9529,7 @@
         <v>0</v>
       </c>
       <c r="AC97">
-        <v>4.95261873828351</v>
+        <v>4.953191580972033</v>
       </c>
     </row>
     <row r="98" spans="1:29">
@@ -9534,7 +9540,7 @@
         <v>55</v>
       </c>
       <c r="C98" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="D98" t="b">
         <v>0</v>
@@ -9612,7 +9618,7 @@
         <v>0</v>
       </c>
       <c r="AC98">
-        <v>5.62543749699015</v>
+        <v>5.625920337168784</v>
       </c>
     </row>
     <row r="99" spans="1:29">
@@ -9623,7 +9629,7 @@
         <v>56</v>
       </c>
       <c r="C99" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="D99" t="b">
         <v>0</v>
@@ -9701,7 +9707,7 @@
         <v>0</v>
       </c>
       <c r="AC99">
-        <v>5.90772716251364</v>
+        <v>5.896963223304297</v>
       </c>
     </row>
     <row r="100" spans="1:29">
@@ -9712,7 +9718,7 @@
         <v>57</v>
       </c>
       <c r="C100" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="D100" t="b">
         <v>0</v>
@@ -9790,7 +9796,7 @@
         <v>2.25</v>
       </c>
       <c r="AC100">
-        <v>5.46931822735864</v>
+        <v>5.458457410138247</v>
       </c>
     </row>
     <row r="101" spans="1:29">
@@ -9801,7 +9807,7 @@
         <v>57</v>
       </c>
       <c r="C101" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="D101" t="b">
         <v>0</v>
@@ -9879,7 +9885,7 @@
         <v>2.25</v>
       </c>
       <c r="AC101">
-        <v>4.97401976241579</v>
+        <v>4.976008653112045</v>
       </c>
     </row>
     <row r="102" spans="1:29">
@@ -9890,7 +9896,7 @@
         <v>57</v>
       </c>
       <c r="C102" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="D102" t="b">
         <v>1</v>
@@ -9968,7 +9974,7 @@
         <v>2.25</v>
       </c>
       <c r="AC102">
-        <v>5.61785456122824</v>
+        <v>5.630688314236976</v>
       </c>
     </row>
     <row r="103" spans="1:29">
@@ -9979,7 +9985,7 @@
         <v>58</v>
       </c>
       <c r="C103" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="D103" t="b">
         <v>1</v>
@@ -10057,7 +10063,7 @@
         <v>2</v>
       </c>
       <c r="AC103">
-        <v>7.54992952251195</v>
+        <v>7.539769353797888</v>
       </c>
     </row>
     <row r="104" spans="1:29">
@@ -10068,7 +10074,7 @@
         <v>58</v>
       </c>
       <c r="C104" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="D104" t="b">
         <v>0</v>
@@ -10146,7 +10152,7 @@
         <v>2</v>
       </c>
       <c r="AC104">
-        <v>6.12394927769071</v>
+        <v>6.112787343966355</v>
       </c>
     </row>
     <row r="105" spans="1:29">
@@ -10157,7 +10163,7 @@
         <v>58</v>
       </c>
       <c r="C105" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="D105" t="b">
         <v>1</v>
@@ -10235,7 +10241,7 @@
         <v>2</v>
       </c>
       <c r="AC105">
-        <v>6.98833957264685</v>
+        <v>7.075846110082174</v>
       </c>
     </row>
     <row r="106" spans="1:29">
@@ -10246,7 +10252,7 @@
         <v>58</v>
       </c>
       <c r="C106" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="D106" t="b">
         <v>0</v>
@@ -10324,7 +10330,7 @@
         <v>2</v>
       </c>
       <c r="AC106">
-        <v>5.46747966044896</v>
+        <v>5.462148723919706</v>
       </c>
     </row>
     <row r="107" spans="1:29">
@@ -10335,7 +10341,7 @@
         <v>58</v>
       </c>
       <c r="C107" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="D107" t="b">
         <v>0</v>
@@ -10413,7 +10419,7 @@
         <v>2</v>
       </c>
       <c r="AC107">
-        <v>3.93677120005074</v>
+        <v>3.961228699695829</v>
       </c>
     </row>
     <row r="108" spans="1:29">
@@ -10424,7 +10430,7 @@
         <v>59</v>
       </c>
       <c r="C108" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="D108" t="b">
         <v>0</v>
@@ -10502,7 +10508,7 @@
         <v>0</v>
       </c>
       <c r="AC108">
-        <v>6.13306652710236</v>
+        <v>6.099282282992595</v>
       </c>
     </row>
     <row r="109" spans="1:29">
@@ -10513,7 +10519,7 @@
         <v>59</v>
       </c>
       <c r="C109" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="D109" t="b">
         <v>0</v>
@@ -10591,7 +10597,7 @@
         <v>0.7</v>
       </c>
       <c r="AC109">
-        <v>6.0023254938974</v>
+        <v>5.968479705860054</v>
       </c>
     </row>
     <row r="110" spans="1:29">
@@ -10602,7 +10608,7 @@
         <v>59</v>
       </c>
       <c r="C110" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="D110" t="b">
         <v>0</v>
@@ -10680,7 +10686,7 @@
         <v>0.7</v>
       </c>
       <c r="AC110">
-        <v>4.68853881466038</v>
+        <v>4.713129710404051</v>
       </c>
     </row>
     <row r="111" spans="1:29">
@@ -10691,7 +10697,7 @@
         <v>59</v>
       </c>
       <c r="C111" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="D111" t="b">
         <v>1</v>
@@ -10769,7 +10775,7 @@
         <v>0.7</v>
       </c>
       <c r="AC111">
-        <v>6.07152679670806</v>
+        <v>6.111126864155356</v>
       </c>
     </row>
     <row r="112" spans="1:29">
@@ -10780,7 +10786,7 @@
         <v>60</v>
       </c>
       <c r="C112" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="D112" t="b">
         <v>0</v>
@@ -10858,7 +10864,7 @@
         <v>0.6</v>
       </c>
       <c r="AC112">
-        <v>6.04632784348829</v>
+        <v>6.048302447522063</v>
       </c>
     </row>
     <row r="113" spans="1:29">
@@ -10869,7 +10875,7 @@
         <v>60</v>
       </c>
       <c r="C113" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="D113" t="b">
         <v>0</v>
@@ -10947,7 +10953,96 @@
         <v>0.5</v>
       </c>
       <c r="AC113">
-        <v>5.7725346020275</v>
+        <v>5.774504519512302</v>
+      </c>
+    </row>
+    <row r="114" spans="1:29">
+      <c r="A114" s="1">
+        <v>112</v>
+      </c>
+      <c r="B114" t="s">
+        <v>61</v>
+      </c>
+      <c r="C114" t="s">
+        <v>174</v>
+      </c>
+      <c r="D114" t="b">
+        <v>1</v>
+      </c>
+      <c r="E114">
+        <v>25</v>
+      </c>
+      <c r="F114">
+        <v>20</v>
+      </c>
+      <c r="G114">
+        <v>74</v>
+      </c>
+      <c r="H114">
+        <v>77</v>
+      </c>
+      <c r="I114">
+        <v>28.25</v>
+      </c>
+      <c r="J114">
+        <v>103</v>
+      </c>
+      <c r="K114">
+        <v>745</v>
+      </c>
+      <c r="L114">
+        <v>168.7</v>
+      </c>
+      <c r="M114">
+        <v>1</v>
+      </c>
+      <c r="N114">
+        <v>6</v>
+      </c>
+      <c r="O114">
+        <v>2</v>
+      </c>
+      <c r="P114">
+        <v>10</v>
+      </c>
+      <c r="Q114">
+        <v>17</v>
+      </c>
+      <c r="R114">
+        <v>63</v>
+      </c>
+      <c r="S114">
+        <v>20</v>
+      </c>
+      <c r="T114">
+        <v>9</v>
+      </c>
+      <c r="U114">
+        <v>68</v>
+      </c>
+      <c r="V114">
+        <v>24123</v>
+      </c>
+      <c r="W114">
+        <v>642</v>
+      </c>
+      <c r="X114">
+        <v>50</v>
+      </c>
+      <c r="Y114">
+        <v>144</v>
+      </c>
+      <c r="Z114">
+        <v>899</v>
+      </c>
+      <c r="AA114">
+        <v>5.75</v>
+      </c>
+      <c r="AB114">
+        <v>5.75</v>
+      </c>
+      <c r="AC114">
+        <v>5.930666430938779</v>
       </c>
     </row>
   </sheetData>

</xml_diff>